<commit_message>
FEATURE Change in sorting in final concat: by date and descending // FEATURE Add index to results file rejected UL numbers to check
</commit_message>
<xml_diff>
--- a/Rejected UL numbers to check.xlsx
+++ b/Rejected UL numbers to check.xlsx
@@ -55,16 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,67 +425,93 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Indeks</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>UL</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Last delivery</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1">
-      <c r="A2" s="3" t="n">
+    <row r="2">
+      <c r="A2" t="n">
+        <v>37221</v>
+      </c>
+      <c r="B2" t="n">
         <v>473221</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>2024-06-25</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1">
-      <c r="A3" s="3" t="n">
-        <v>248209</v>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>2024-05-27</t>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>56138</v>
+      </c>
+      <c r="B3" t="n">
+        <v>345919</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-12-03</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1">
-      <c r="A4" s="3" t="n">
-        <v>340369</v>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>2024-03-05</t>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>55472</v>
+      </c>
+      <c r="B4" t="n">
+        <v>132781</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="30" customHeight="1">
-      <c r="A5" s="3" t="n">
-        <v>28603</v>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>2024-05-14</t>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>59958</v>
+      </c>
+      <c r="B5" t="n">
+        <v>174211</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>60988</v>
+      </c>
+      <c r="B6" t="n">
+        <v>360486</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
         </is>
       </c>
     </row>

</xml_diff>